<commit_message>
actualizacion y subida de script
</commit_message>
<xml_diff>
--- a/Output/reportes_2025-08-24.xlsx
+++ b/Output/reportes_2025-08-24.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="108">
   <si>
     <t xml:space="preserve">id </t>
   </si>
@@ -332,6 +332,18 @@
   </si>
   <si>
     <t xml:space="preserve">8/24/2025 12:49:27 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8/24/2025 1:35:52 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8/24/2025 1:50:55 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8/24/2025 1:56:36 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8/24/2025 2:05:21 AM</t>
   </si>
 </sst>
 </file>
@@ -738,7 +750,7 @@
         <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G2"/>
     </row>
@@ -759,7 +771,7 @@
         <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G3"/>
     </row>
@@ -780,7 +792,7 @@
         <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G4"/>
     </row>
@@ -801,7 +813,7 @@
         <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G5"/>
     </row>
@@ -822,7 +834,7 @@
         <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G6"/>
     </row>
@@ -843,7 +855,7 @@
         <v>39</v>
       </c>
       <c r="F7" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G7"/>
     </row>
@@ -864,7 +876,7 @@
         <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G8"/>
     </row>
@@ -885,7 +897,7 @@
         <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G9"/>
     </row>
@@ -906,7 +918,7 @@
         <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G10"/>
     </row>
@@ -927,7 +939,7 @@
         <v>56</v>
       </c>
       <c r="F11" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G11"/>
     </row>
@@ -948,7 +960,7 @@
         <v>59</v>
       </c>
       <c r="F12" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G12"/>
     </row>
@@ -969,7 +981,7 @@
         <v>63</v>
       </c>
       <c r="F13" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G13"/>
     </row>
@@ -990,7 +1002,7 @@
         <v>67</v>
       </c>
       <c r="F14" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G14"/>
     </row>
@@ -1011,7 +1023,7 @@
         <v>71</v>
       </c>
       <c r="F15" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G15"/>
     </row>
@@ -1032,7 +1044,7 @@
         <v>76</v>
       </c>
       <c r="F16" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G16"/>
     </row>
@@ -1053,7 +1065,7 @@
         <v>80</v>
       </c>
       <c r="F17" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G17"/>
     </row>
@@ -1074,7 +1086,7 @@
         <v>84</v>
       </c>
       <c r="F18" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G18"/>
     </row>
@@ -1095,7 +1107,7 @@
         <v>88</v>
       </c>
       <c r="F19" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G19"/>
     </row>
@@ -1116,7 +1128,7 @@
         <v>92</v>
       </c>
       <c r="F20" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G20"/>
     </row>
@@ -1137,7 +1149,7 @@
         <v>96</v>
       </c>
       <c r="F21" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G21"/>
     </row>

</xml_diff>